<commit_message>
weighted average only for proxies
</commit_message>
<xml_diff>
--- a/data/interim/fully-covered-definition_2020-05-31.xlsx
+++ b/data/interim/fully-covered-definition_2020-05-31.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,15 +379,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>proxy_score</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>stateness</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>successful_transition</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>approach</t>
         </is>
@@ -403,12 +408,15 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>45.7365810402868</v>
+        <v>7.34216935367578</v>
       </c>
       <c r="D2" t="n">
+        <v>91.77711692094725</v>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>fully covered</t>
         </is>
@@ -424,12 +432,15 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>21.96329636627423</v>
+        <v>3.475321885018063</v>
       </c>
       <c r="D3" t="n">
+        <v>43.44152356272578</v>
+      </c>
+      <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>fully covered</t>
         </is>
@@ -445,12 +456,15 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>27.76221807586535</v>
+        <v>4.718378336635055</v>
       </c>
       <c r="D4" t="n">
+        <v>58.97972920793819</v>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>fully covered</t>
         </is>
@@ -466,12 +480,15 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>13.35578205968594</v>
+        <v>2.189408382985685</v>
       </c>
       <c r="D5" t="n">
+        <v>27.36760478732106</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>fully covered</t>
         </is>
@@ -487,12 +504,15 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>14.58655421043453</v>
+        <v>2.429787986552066</v>
       </c>
       <c r="D6" t="n">
+        <v>30.37234983190082</v>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>fully covered</t>
         </is>
@@ -508,12 +528,15 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14.01313459748565</v>
+        <v>2.273261133685839</v>
       </c>
       <c r="D7" t="n">
+        <v>28.41576417107299</v>
+      </c>
+      <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>fully covered</t>
         </is>
@@ -529,12 +552,15 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>27.52887012596806</v>
+        <v>4.681216693802947</v>
       </c>
       <c r="D8" t="n">
+        <v>58.51520867253684</v>
+      </c>
+      <c r="E8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>fully covered</t>
         </is>

</xml_diff>